<commit_message>
fixing the excel bug NaN on the server side and start new featcher ReExam
</commit_message>
<xml_diff>
--- a/api/UPLOAD_FOLDER/Book4.xlsx
+++ b/api/UPLOAD_FOLDER/Book4.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAA7AA0C-8901-45C0-8E83-76EE2BF74300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Louie\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD668CA0-832C-40B8-83A1-5120543266A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{46D29571-D7D8-4D0C-9C07-159198B5069F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{46D29571-D7D8-4D0C-9C07-159198B5069F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="14">
   <si>
     <t>Student Group</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -72,7 +77,13 @@
     <t>Shift</t>
   </si>
   <si>
-    <t>Group-01</t>
+    <t>SOL3-C94-2023</t>
+  </si>
+  <si>
+    <t>SOL3-C95-2023</t>
+  </si>
+  <si>
+    <t>SOL3-C99-2023</t>
   </si>
 </sst>
 </file>
@@ -7324,26 +7335,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DDF099-F64E-4BB1-BBAE-08D61AD63CA5}">
   <dimension ref="A1:K232"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="B219" sqref="B219"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="2" max="2" width="68.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7378,7 +7389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -7422,7 +7433,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -7466,7 +7477,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -7510,7 +7521,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -7554,7 +7565,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -7598,7 +7609,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -7642,7 +7653,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -7686,7 +7697,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -7730,7 +7741,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -7774,7 +7785,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -7818,7 +7829,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -7862,7 +7873,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -7906,7 +7917,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -7950,7 +7961,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -7994,7 +8005,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
@@ -8038,7 +8049,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
@@ -8082,7 +8093,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
@@ -8126,7 +8137,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
@@ -8170,7 +8181,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
@@ -8214,7 +8225,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>11</v>
       </c>
@@ -8258,7 +8269,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>11</v>
       </c>
@@ -8302,7 +8313,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
@@ -8346,7 +8357,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>11</v>
       </c>
@@ -8390,7 +8401,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>11</v>
       </c>
@@ -8434,7 +8445,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>11</v>
       </c>
@@ -8478,7 +8489,7 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>11</v>
       </c>
@@ -8522,9 +8533,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B28" s="4" t="str">
         <f>[1]DATA!C28</f>
@@ -8566,9 +8577,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B29" s="4" t="str">
         <f>[1]DATA!C29</f>
@@ -8610,9 +8621,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B30" s="4" t="str">
         <f>[1]DATA!C30</f>
@@ -8654,9 +8665,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B31" s="4" t="str">
         <f>[1]DATA!C31</f>
@@ -8698,9 +8709,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B32" s="4" t="str">
         <f>[1]DATA!C32</f>
@@ -8742,9 +8753,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B33" s="4" t="str">
         <f>[1]DATA!C33</f>
@@ -8786,9 +8797,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B34" s="4" t="str">
         <f>[1]DATA!C34</f>
@@ -8830,9 +8841,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B35" s="4" t="str">
         <f>[1]DATA!C35</f>
@@ -8874,9 +8885,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B36" s="4" t="str">
         <f>[1]DATA!C36</f>
@@ -8918,9 +8929,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B37" s="4" t="str">
         <f>[1]DATA!C37</f>
@@ -8962,9 +8973,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B38" s="4" t="str">
         <f>[1]DATA!C38</f>
@@ -9006,9 +9017,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B39" s="4" t="str">
         <f>[1]DATA!C39</f>
@@ -9050,9 +9061,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B40" s="4" t="str">
         <f>[1]DATA!C40</f>
@@ -9094,9 +9105,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B41" s="4" t="str">
         <f>[1]DATA!C41</f>
@@ -9138,9 +9149,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B42" s="4" t="str">
         <f>[1]DATA!C42</f>
@@ -9182,9 +9193,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B43" s="4" t="str">
         <f>[1]DATA!C43</f>
@@ -9226,9 +9237,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B44" s="4" t="str">
         <f>[1]DATA!C44</f>
@@ -9270,9 +9281,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B45" s="4" t="str">
         <f>[1]DATA!C45</f>
@@ -9314,9 +9325,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B46" s="4" t="str">
         <f>[1]DATA!C46</f>
@@ -9358,9 +9369,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B47" s="4" t="str">
         <f>[1]DATA!C47</f>
@@ -9402,9 +9413,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B48" s="4" t="str">
         <f>[1]DATA!C48</f>
@@ -9446,9 +9457,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B49" s="4" t="str">
         <f>[1]DATA!C49</f>
@@ -9490,9 +9501,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B50" s="4" t="str">
         <f>[1]DATA!C50</f>
@@ -9534,9 +9545,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B51" s="4" t="str">
         <f>[1]DATA!C51</f>
@@ -9578,9 +9589,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B52" s="4" t="str">
         <f>[1]DATA!C52</f>
@@ -9622,9 +9633,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B53" s="4" t="str">
         <f>[1]DATA!C53</f>
@@ -9666,9 +9677,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B54" s="4" t="str">
         <f>[1]DATA!C54</f>
@@ -9710,9 +9721,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B55" s="4" t="str">
         <f>[1]DATA!C55</f>
@@ -9754,9 +9765,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B56" s="4" t="str">
         <f>[1]DATA!C56</f>
@@ -9798,9 +9809,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B57" s="4" t="str">
         <f>[1]DATA!C57</f>
@@ -9842,9 +9853,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B58" s="4" t="str">
         <f>[1]DATA!C58</f>
@@ -9886,9 +9897,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B59" s="4" t="str">
         <f>[1]DATA!C59</f>
@@ -9930,9 +9941,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B60" s="4" t="str">
         <f>[1]DATA!C60</f>
@@ -9974,9 +9985,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B61" s="4" t="str">
         <f>[1]DATA!C61</f>
@@ -10018,9 +10029,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B62" s="4" t="str">
         <f>[1]DATA!C62</f>
@@ -10062,9 +10073,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B63" s="4" t="str">
         <f>[1]DATA!C63</f>
@@ -10106,9 +10117,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B64" s="4" t="str">
         <f>[1]DATA!C64</f>
@@ -10150,9 +10161,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B65" s="4" t="str">
         <f>[1]DATA!C65</f>
@@ -10194,9 +10205,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B66" s="4" t="str">
         <f>[1]DATA!C66</f>
@@ -10238,9 +10249,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B67" s="4" t="str">
         <f>[1]DATA!C67</f>
@@ -10282,9 +10293,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B68" s="4" t="str">
         <f>[1]DATA!C68</f>
@@ -10326,9 +10337,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B69" s="4" t="str">
         <f>[1]DATA!C69</f>
@@ -10370,9 +10381,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B70" s="4" t="str">
         <f>[1]DATA!C70</f>
@@ -10414,9 +10425,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B71" s="4" t="str">
         <f>[1]DATA!C71</f>
@@ -10458,9 +10469,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B72" s="4" t="str">
         <f>[1]DATA!C72</f>
@@ -10502,9 +10513,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B73" s="4" t="str">
         <f>[1]DATA!C73</f>
@@ -10546,9 +10557,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B74" s="4" t="str">
         <f>[1]DATA!C74</f>
@@ -10590,9 +10601,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B75" s="4" t="str">
         <f>[1]DATA!C75</f>
@@ -10634,9 +10645,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B76" s="4" t="str">
         <f>[1]DATA!C76</f>
@@ -10678,9 +10689,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B77" s="4" t="str">
         <f>[1]DATA!C77</f>
@@ -10722,9 +10733,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B78" s="4" t="str">
         <f>[1]DATA!C78</f>
@@ -10766,9 +10777,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B79" s="4" t="str">
         <f>[1]DATA!C79</f>
@@ -10810,9 +10821,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B80" s="4" t="str">
         <f>[1]DATA!C80</f>
@@ -10854,9 +10865,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B81" s="4" t="str">
         <f>[1]DATA!C81</f>
@@ -10898,9 +10909,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B82" s="4" t="str">
         <f>[1]DATA!C82</f>
@@ -10942,9 +10953,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B83" s="4" t="str">
         <f>[1]DATA!C83</f>
@@ -10986,9 +10997,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B84" s="4" t="str">
         <f>[1]DATA!C84</f>
@@ -11030,9 +11041,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B85" s="4" t="str">
         <f>[1]DATA!C85</f>
@@ -11074,9 +11085,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B86" s="4" t="str">
         <f>[1]DATA!C86</f>
@@ -11118,9 +11129,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B87" s="4" t="str">
         <f>[1]DATA!C87</f>
@@ -11162,9 +11173,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B88" s="4" t="str">
         <f>[1]DATA!C88</f>
@@ -11206,9 +11217,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B89" s="4" t="str">
         <f>[1]DATA!C89</f>
@@ -11250,9 +11261,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B90" s="4" t="str">
         <f>[1]DATA!C90</f>
@@ -11294,9 +11305,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B91" s="4" t="str">
         <f>[1]DATA!C91</f>
@@ -11338,9 +11349,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B92" s="4" t="str">
         <f>[1]DATA!C92</f>
@@ -11382,9 +11393,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B93" s="4" t="str">
         <f>[1]DATA!C93</f>
@@ -11426,9 +11437,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B94" s="4" t="str">
         <f>[1]DATA!C94</f>
@@ -11470,9 +11481,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B95" s="4" t="str">
         <f>[1]DATA!C95</f>
@@ -11514,9 +11525,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B96" s="4" t="str">
         <f>[1]DATA!C96</f>
@@ -11558,9 +11569,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B97" s="4" t="str">
         <f>[1]DATA!C97</f>
@@ -11602,9 +11613,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B98" s="4" t="str">
         <f>[1]DATA!C98</f>
@@ -11646,9 +11657,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B99" s="4" t="str">
         <f>[1]DATA!C99</f>
@@ -11690,9 +11701,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B100" s="4" t="str">
         <f>[1]DATA!C100</f>
@@ -11734,9 +11745,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B101" s="4" t="str">
         <f>[1]DATA!C101</f>
@@ -11778,9 +11789,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B102" s="4" t="str">
         <f>[1]DATA!C102</f>
@@ -11822,9 +11833,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B103" s="4" t="str">
         <f>[1]DATA!C103</f>
@@ -11866,9 +11877,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B104" s="4" t="str">
         <f>[1]DATA!C104</f>
@@ -11910,9 +11921,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B105" s="4" t="str">
         <f>[1]DATA!C105</f>
@@ -11954,9 +11965,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B106" s="4" t="str">
         <f>[1]DATA!C106</f>
@@ -11998,9 +12009,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B107" s="4" t="str">
         <f>[1]DATA!C107</f>
@@ -12042,9 +12053,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B108" s="4" t="str">
         <f>[1]DATA!C108</f>
@@ -12086,9 +12097,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B109" s="4" t="str">
         <f>[1]DATA!C109</f>
@@ -12130,9 +12141,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B110" s="4" t="str">
         <f>[1]DATA!C110</f>
@@ -12174,9 +12185,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B111" s="4" t="str">
         <f>[1]DATA!C111</f>
@@ -12218,9 +12229,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B112" s="4" t="str">
         <f>[1]DATA!C112</f>
@@ -12262,9 +12273,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B113" s="4" t="str">
         <f>[1]DATA!C113</f>
@@ -12306,9 +12317,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B114" s="4" t="str">
         <f>[1]DATA!C114</f>
@@ -12350,9 +12361,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B115" s="4" t="str">
         <f>[1]DATA!C115</f>
@@ -12394,9 +12405,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B116" s="4" t="str">
         <f>[1]DATA!C116</f>
@@ -12438,9 +12449,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B117" s="4" t="str">
         <f>[1]DATA!C117</f>
@@ -12482,9 +12493,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B118" s="4" t="str">
         <f>[1]DATA!C118</f>
@@ -12526,9 +12537,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B119" s="4" t="str">
         <f>[1]DATA!C119</f>
@@ -12570,9 +12581,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B120" s="4" t="str">
         <f>[1]DATA!C120</f>
@@ -12614,9 +12625,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B121" s="4" t="str">
         <f>[1]DATA!C121</f>
@@ -12658,9 +12669,9 @@
         <v>Evening</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B122" s="4" t="str">
         <f>[1]DATA!C122</f>
@@ -12702,9 +12713,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B123" s="4" t="str">
         <f>[1]DATA!C123</f>
@@ -12746,9 +12757,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B124" s="4" t="str">
         <f>[1]DATA!C124</f>
@@ -12790,9 +12801,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B125" s="4" t="str">
         <f>[1]DATA!C125</f>
@@ -12834,9 +12845,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B126" s="4" t="str">
         <f>[1]DATA!C126</f>
@@ -12878,9 +12889,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A127" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B127" s="4" t="str">
         <f>[1]DATA!C127</f>
@@ -12922,9 +12933,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B128" s="4" t="str">
         <f>[1]DATA!C128</f>
@@ -12966,9 +12977,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B129" s="4" t="str">
         <f>[1]DATA!C129</f>
@@ -13010,9 +13021,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="130" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B130" s="4" t="str">
         <f>[1]DATA!C130</f>
@@ -13054,9 +13065,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="131" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B131" s="4" t="str">
         <f>[1]DATA!C131</f>
@@ -13098,9 +13109,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="132" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B132" s="4" t="str">
         <f>[1]DATA!C132</f>
@@ -13142,9 +13153,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="133" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B133" s="4" t="str">
         <f>[1]DATA!C133</f>
@@ -13186,9 +13197,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="134" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B134" s="4" t="str">
         <f>[1]DATA!C134</f>
@@ -13230,9 +13241,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="135" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B135" s="4" t="str">
         <f>[1]DATA!C135</f>
@@ -13274,9 +13285,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="136" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B136" s="4" t="str">
         <f>[1]DATA!C136</f>
@@ -13318,9 +13329,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B137" s="4" t="str">
         <f>[1]DATA!C137</f>
@@ -13362,9 +13373,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B138" s="4" t="str">
         <f>[1]DATA!C138</f>
@@ -13406,9 +13417,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="139" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B139" s="4" t="str">
         <f>[1]DATA!C139</f>
@@ -13450,9 +13461,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="140" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B140" s="4" t="str">
         <f>[1]DATA!C140</f>
@@ -13494,9 +13505,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B141" s="4" t="str">
         <f>[1]DATA!C141</f>
@@ -13538,9 +13549,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="142" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B142" s="4" t="str">
         <f>[1]DATA!C142</f>
@@ -13582,9 +13593,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A143" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B143" s="4" t="str">
         <f>[1]DATA!C143</f>
@@ -13626,9 +13637,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="144" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B144" s="4" t="str">
         <f>[1]DATA!C144</f>
@@ -13670,9 +13681,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="145" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A145" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B145" s="4" t="str">
         <f>[1]DATA!C145</f>
@@ -13714,9 +13725,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B146" s="4" t="str">
         <f>[1]DATA!C146</f>
@@ -13758,9 +13769,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="147" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B147" s="4" t="str">
         <f>[1]DATA!C147</f>
@@ -13802,9 +13813,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="148" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A148" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B148" s="4" t="str">
         <f>[1]DATA!C148</f>
@@ -13846,9 +13857,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="149" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A149" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B149" s="4" t="str">
         <f>[1]DATA!C149</f>
@@ -13890,9 +13901,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="150" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A150" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B150" s="4" t="str">
         <f>[1]DATA!C150</f>
@@ -13934,9 +13945,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="151" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A151" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B151" s="4" t="str">
         <f>[1]DATA!C151</f>
@@ -13978,9 +13989,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A152" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B152" s="4" t="str">
         <f>[1]DATA!C152</f>
@@ -14022,9 +14033,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="153" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A153" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B153" s="4" t="str">
         <f>[1]DATA!C153</f>
@@ -14066,9 +14077,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="154" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A154" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B154" s="4" t="str">
         <f>[1]DATA!C154</f>
@@ -14110,9 +14121,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A155" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B155" s="4" t="str">
         <f>[1]DATA!C155</f>
@@ -14154,9 +14165,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A156" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B156" s="4" t="str">
         <f>[1]DATA!C156</f>
@@ -14198,9 +14209,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="157" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A157" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B157" s="4" t="str">
         <f>[1]DATA!C157</f>
@@ -14242,9 +14253,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="158" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A158" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B158" s="4" t="str">
         <f>[1]DATA!C158</f>
@@ -14286,9 +14297,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A159" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B159" s="4" t="str">
         <f>[1]DATA!C159</f>
@@ -14330,9 +14341,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="160" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A160" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B160" s="4" t="str">
         <f>[1]DATA!C160</f>
@@ -14374,9 +14385,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="161" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A161" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B161" s="4" t="str">
         <f>[1]DATA!C161</f>
@@ -14418,9 +14429,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="162" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A162" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B162" s="4" t="str">
         <f>[1]DATA!C162</f>
@@ -14462,9 +14473,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A163" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B163" s="4" t="str">
         <f>[1]DATA!C163</f>
@@ -14506,9 +14517,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A164" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B164" s="4" t="str">
         <f>[1]DATA!C164</f>
@@ -14550,9 +14561,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A165" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B165" s="4" t="str">
         <f>[1]DATA!C165</f>
@@ -14594,9 +14605,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A166" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B166" s="4" t="str">
         <f>[1]DATA!C166</f>
@@ -14638,9 +14649,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A167" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B167" s="4" t="str">
         <f>[1]DATA!C167</f>
@@ -14682,9 +14693,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A168" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B168" s="4" t="str">
         <f>[1]DATA!C168</f>
@@ -14726,9 +14737,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A169" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B169" s="4" t="str">
         <f>[1]DATA!C169</f>
@@ -14770,9 +14781,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="170" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A170" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B170" s="4" t="str">
         <f>[1]DATA!C170</f>
@@ -14814,9 +14825,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="171" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A171" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B171" s="4" t="str">
         <f>[1]DATA!C171</f>
@@ -14858,9 +14869,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="172" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A172" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B172" s="4" t="str">
         <f>[1]DATA!C172</f>
@@ -14902,9 +14913,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A173" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B173" s="4" t="str">
         <f>[1]DATA!C173</f>
@@ -14946,9 +14957,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A174" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B174" s="4" t="str">
         <f>[1]DATA!C174</f>
@@ -14990,9 +15001,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="175" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A175" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B175" s="4" t="str">
         <f>[1]DATA!C175</f>
@@ -15034,9 +15045,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="176" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A176" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B176" s="4" t="str">
         <f>[1]DATA!C176</f>
@@ -15078,9 +15089,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="177" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A177" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B177" s="4" t="str">
         <f>[1]DATA!C177</f>
@@ -15122,9 +15133,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="178" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A178" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B178" s="4" t="str">
         <f>[1]DATA!C178</f>
@@ -15166,9 +15177,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="179" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A179" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B179" s="4" t="str">
         <f>[1]DATA!C179</f>
@@ -15210,9 +15221,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="180" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A180" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B180" s="4" t="str">
         <f>[1]DATA!C180</f>
@@ -15254,9 +15265,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A181" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B181" s="4" t="str">
         <f>[1]DATA!C181</f>
@@ -15298,9 +15309,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="182" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A182" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B182" s="4" t="str">
         <f>[1]DATA!C182</f>
@@ -15342,9 +15353,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="183" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A183" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B183" s="4" t="str">
         <f>[1]DATA!C183</f>
@@ -15386,9 +15397,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="184" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A184" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B184" s="4" t="str">
         <f>[1]DATA!C184</f>
@@ -15430,9 +15441,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="185" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A185" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B185" s="4" t="str">
         <f>[1]DATA!C185</f>
@@ -15474,9 +15485,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="186" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A186" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B186" s="4" t="str">
         <f>[1]DATA!C186</f>
@@ -15518,9 +15529,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="187" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A187" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B187" s="4" t="str">
         <f>[1]DATA!C187</f>
@@ -15562,9 +15573,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="188" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A188" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B188" s="4" t="str">
         <f>[1]DATA!C188</f>
@@ -15606,9 +15617,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="189" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A189" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B189" s="4" t="str">
         <f>[1]DATA!C189</f>
@@ -15650,9 +15661,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="190" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A190" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B190" s="4" t="str">
         <f>[1]DATA!C190</f>
@@ -15694,9 +15705,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="191" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A191" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B191" s="4" t="str">
         <f>[1]DATA!C191</f>
@@ -15738,9 +15749,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="192" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A192" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B192" s="4" t="str">
         <f>[1]DATA!C192</f>
@@ -15782,9 +15793,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A193" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B193" s="4" t="str">
         <f>[1]DATA!C193</f>
@@ -15826,9 +15837,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="194" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A194" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B194" s="4" t="str">
         <f>[1]DATA!C194</f>
@@ -15870,9 +15881,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="195" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A195" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B195" s="4" t="str">
         <f>[1]DATA!C195</f>
@@ -15914,9 +15925,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="196" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A196" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B196" s="4" t="str">
         <f>[1]DATA!C196</f>
@@ -15958,9 +15969,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="197" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A197" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B197" s="4" t="str">
         <f>[1]DATA!C197</f>
@@ -16002,9 +16013,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="198" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A198" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B198" s="4" t="str">
         <f>[1]DATA!C198</f>
@@ -16046,9 +16057,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="199" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A199" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B199" s="4" t="str">
         <f>[1]DATA!C199</f>
@@ -16090,9 +16101,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="200" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A200" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B200" s="4" t="str">
         <f>[1]DATA!C200</f>
@@ -16134,9 +16145,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="201" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A201" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B201" s="4" t="str">
         <f>[1]DATA!C201</f>
@@ -16178,9 +16189,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="202" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A202" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B202" s="4" t="str">
         <f>[1]DATA!C202</f>
@@ -16222,9 +16233,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="203" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A203" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B203" s="4" t="str">
         <f>[1]DATA!C203</f>
@@ -16266,9 +16277,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="204" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A204" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B204" s="4" t="str">
         <f>[1]DATA!C204</f>
@@ -16310,9 +16321,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="205" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A205" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B205" s="4" t="str">
         <f>[1]DATA!C205</f>
@@ -16354,9 +16365,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="206" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A206" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B206" s="4" t="str">
         <f>[1]DATA!C206</f>
@@ -16398,9 +16409,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="207" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A207" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B207" s="4" t="str">
         <f>[1]DATA!C207</f>
@@ -16442,9 +16453,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="208" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A208" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B208" s="4" t="str">
         <f>[1]DATA!C208</f>
@@ -16486,9 +16497,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="209" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A209" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B209" s="4" t="str">
         <f>[1]DATA!C209</f>
@@ -16530,9 +16541,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="210" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A210" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B210" s="4" t="str">
         <f>[1]DATA!C210</f>
@@ -16574,9 +16585,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="211" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A211" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B211" s="4" t="str">
         <f>[1]DATA!C211</f>
@@ -16618,9 +16629,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="212" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A212" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B212" s="4" t="str">
         <f>[1]DATA!C212</f>
@@ -16662,9 +16673,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="213" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A213" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B213" s="4" t="str">
         <f>[1]DATA!C213</f>
@@ -16706,9 +16717,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="214" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A214" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B214" s="4" t="str">
         <f>[1]DATA!C214</f>
@@ -16750,9 +16761,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="215" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A215" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B215" s="4" t="str">
         <f>[1]DATA!C215</f>
@@ -16794,9 +16805,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="216" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A216" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B216" s="4" t="str">
         <f>[1]DATA!C216</f>
@@ -16838,9 +16849,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="217" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A217" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B217" s="4" t="str">
         <f>[1]DATA!C217</f>
@@ -16882,9 +16893,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="218" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A218" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B218" s="4" t="str">
         <f>[1]DATA!C218</f>
@@ -16926,9 +16937,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="219" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A219" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B219" s="4" t="str">
         <f>[1]DATA!C219</f>
@@ -16970,9 +16981,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="220" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A220" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B220" s="4" t="str">
         <f>[1]DATA!C220</f>
@@ -17014,9 +17025,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="221" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A221" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B221" s="4" t="str">
         <f>[1]DATA!C221</f>
@@ -17058,9 +17069,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="222" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A222" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B222" s="4" t="str">
         <f>[1]DATA!C222</f>
@@ -17102,9 +17113,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="223" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A223" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B223" s="4" t="str">
         <f>[1]DATA!C223</f>
@@ -17146,9 +17157,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="224" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A224" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B224" s="4" t="str">
         <f>[1]DATA!C224</f>
@@ -17190,9 +17201,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="225" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A225" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B225" s="4" t="str">
         <f>[1]DATA!C225</f>
@@ -17234,9 +17245,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="226" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A226" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B226" s="4" t="str">
         <f>[1]DATA!C226</f>
@@ -17278,9 +17289,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="227" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A227" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B227" s="4" t="str">
         <f>[1]DATA!C227</f>
@@ -17322,9 +17333,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="228" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A228" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B228" s="4" t="str">
         <f>[1]DATA!C228</f>
@@ -17366,9 +17377,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="229" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A229" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B229" s="4" t="str">
         <f>[1]DATA!C229</f>
@@ -17410,9 +17421,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="230" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A230" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B230" s="4" t="str">
         <f>[1]DATA!C230</f>
@@ -17454,9 +17465,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="231" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A231" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B231" s="4" t="str">
         <f>[1]DATA!C231</f>
@@ -17498,9 +17509,9 @@
         <v>Morning</v>
       </c>
     </row>
-    <row r="232" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A232" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B232" s="4" t="str">
         <f>[1]DATA!C232</f>

</xml_diff>